<commit_message>
template index fix, searching in dvp fixed
</commit_message>
<xml_diff>
--- a/src/excely/dummy.xlsx
+++ b/src/excely/dummy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukas\Documents\Zimny semester (3)\TIS\github\form-versions\src\excely\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\3AIN\TIS\GITHAB\form-versions\src\excely\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F108DAB6-508E-4E08-BAE8-09B54F47F52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F611CA-C773-4016-B6DE-F6DDC894F0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B16243E4-A542-436E-A4FC-910D7B9A9EF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B16243E4-A542-436E-A4FC-910D7B9A9EF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,6 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -50,12 +46,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -70,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -386,14 +389,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51695196-2C5B-4A97-9041-EE563E23AC28}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T4" s="1"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T22" s="1"/>
+    </row>
+    <row r="23" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T23" s="1"/>
+    </row>
+    <row r="24" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="20:20" x14ac:dyDescent="0.3">
+      <c r="T26" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>